<commit_message>
Made melee attack better Improved logic and flexibility for touch object detection
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder Dungeon World 2.xlsx
+++ b/darkworld/model/data/floor builder Dungeon World 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CACF9FD-E30C-4D80-B657-FD723FC760B0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5F9CD3-085A-4670-9673-6334BF15CB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="1560" windowWidth="22365" windowHeight="15840" tabRatio="904" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11130" yWindow="1560" windowWidth="22365" windowHeight="15840" tabRatio="904" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="70">
   <si>
     <t>width</t>
   </si>
@@ -469,9 +469,6 @@
   </si>
   <si>
     <t>s</t>
-  </si>
-  <si>
-    <t>~</t>
   </si>
 </sst>
 </file>
@@ -3030,8 +3027,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30439A0C-B9B0-4751-993E-75FEF8030A87}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4043,7 +4040,7 @@
         <v>4</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>4</v>
+        <v>35</v>
       </c>
       <c r="J14" s="12" t="s">
         <v>30</v>
@@ -4085,11 +4082,11 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v>#    :   :    :    #</v>
+        <v>#    :  K:    :    #</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'#    :   :    :    #',</v>
+        <v>'#    :  K:    :    #',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -6497,7 +6494,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6810,7 +6807,7 @@
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B5" s="12" t="s">
         <v>4</v>
@@ -6876,16 +6873,16 @@
       <c r="Y5" s="7"/>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">#                   </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'#                   ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B6" s="12" t="s">
         <v>4</v>
@@ -6951,19 +6948,19 @@
       <c r="Y6" s="7"/>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">#                   </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'#                   ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B7" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>4</v>
@@ -7026,11 +7023,11 @@
       <c r="Y7" s="7"/>
       <c r="AA7" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">b#                  </v>
       </c>
       <c r="AB7" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'b#                  ',</v>
       </c>
     </row>
     <row r="8" spans="1:28" x14ac:dyDescent="0.25">
@@ -7485,10 +7482,10 @@
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
-        <v>4</v>
+        <v>37</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>4</v>
@@ -7551,16 +7548,16 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">b#                  </v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'b#                  ',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B15" s="12" t="s">
         <v>4</v>
@@ -7626,16 +7623,16 @@
       <c r="Y15" s="7"/>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">#                   </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'#                   ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>4</v>
+        <v>26</v>
       </c>
       <c r="B16" s="12" t="s">
         <v>4</v>
@@ -7701,11 +7698,11 @@
       <c r="Y16" s="7"/>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">#                   </v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'#                   ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -8230,7 +8227,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA20"/>
+      <selection activeCell="C5" sqref="C5:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8546,7 +8543,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>4</v>
@@ -8609,11 +8606,11 @@
       <c r="Y5" s="7"/>
       <c r="AA5" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve"> *                  </v>
       </c>
       <c r="AB5" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>' *                  ',</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
@@ -8621,7 +8618,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>4</v>
@@ -8684,11 +8681,11 @@
       <c r="Y6" s="7"/>
       <c r="AA6" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve"> *                  </v>
       </c>
       <c r="AB6" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>' *                  ',</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.25">
@@ -9296,7 +9293,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>4</v>
@@ -9359,11 +9356,11 @@
       <c r="Y15" s="7"/>
       <c r="AA15" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve"> *                  </v>
       </c>
       <c r="AB15" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>' *                  ',</v>
       </c>
     </row>
     <row r="16" spans="1:28" x14ac:dyDescent="0.25">
@@ -9371,13 +9368,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D16" s="12" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="E16" s="12" t="s">
         <v>4</v>
@@ -9434,11 +9431,11 @@
       <c r="Y16" s="7"/>
       <c r="AA16" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve"> ***                </v>
       </c>
       <c r="AB16" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>' ***                ',</v>
       </c>
     </row>
     <row r="17" spans="1:28" x14ac:dyDescent="0.25">
@@ -13429,7 +13426,7 @@
   <dimension ref="A1:AB30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AA1" sqref="AA1:AA20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17583,7 +17580,7 @@
     </row>
     <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>4</v>
@@ -17649,16 +17646,16 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v>#                  k</v>
+        <v xml:space="preserve">                   k</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>'#                  k',</v>
+        <v>'                   k',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
-        <v>26</v>
+        <v>4</v>
       </c>
       <c r="B11" s="12" t="s">
         <v>4</v>
@@ -17724,11 +17721,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">#                   </v>
+        <v xml:space="preserve">                    </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'#                   ',</v>
+        <v>'                    ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -17829,22 +17826,22 @@
         <v>26</v>
       </c>
       <c r="H13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L13" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="M13" s="12" t="s">
         <v>67</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="K13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>4</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>4</v>
       </c>
       <c r="N13" s="12" t="s">
         <v>26</v>
@@ -17874,11 +17871,11 @@
       <c r="Y13" s="7"/>
       <c r="AA13" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">#   # #c     ##     </v>
+        <v xml:space="preserve">#   # #     c##     </v>
       </c>
       <c r="AB13" t="str">
         <f t="shared" si="1"/>
-        <v>'#   # #c     ##     ',</v>
+        <v>'#   # #     c##     ',</v>
       </c>
     </row>
     <row r="14" spans="1:28" x14ac:dyDescent="0.25">
@@ -18627,8 +18624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EE1C29-EB6B-4425-BBBF-BA7C396F9AF9}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P11" sqref="P11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19361,13 +19358,13 @@
         <v>24</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="S10" s="12" t="s">
         <v>24</v>
@@ -19382,11 +19379,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> FFFFFFFFFFFFFF~~~FF</v>
+        <v xml:space="preserve"> FFFFFFFFFFFFFF___FF</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>' FFFFFFFFFFFFFF~~~FF',</v>
+        <v>' FFFFFFFFFFFFFF___FF',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -19436,13 +19433,13 @@
         <v>24</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="S11" s="12" t="s">
         <v>24</v>
@@ -19457,11 +19454,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> FFFFFFFFFFFFFF~~~FF</v>
+        <v xml:space="preserve"> FFFFFFFFFFFFFF___FF</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>' FFFFFFFFFFFFFF~~~FF',</v>
+        <v>' FFFFFFFFFFFFFF___FF',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added extra state once your complete a world you then need to press SPACE to go onto teh next world
</commit_message>
<xml_diff>
--- a/darkworld/model/data/floor builder Dungeon World 2.xlsx
+++ b/darkworld/model/data/floor builder Dungeon World 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Development\Python\DarkWorld\darkworld\model\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5F9CD3-085A-4670-9673-6334BF15CB6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DF95735-1E1F-4E76-B85C-5F35C1139319}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11130" yWindow="1560" windowWidth="22365" windowHeight="15840" tabRatio="904" firstSheet="8" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11130" yWindow="1560" windowWidth="22365" windowHeight="15840" tabRatio="904" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blank" sheetId="49" r:id="rId1"/>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7716" uniqueCount="72">
   <si>
     <t>width</t>
   </si>
@@ -469,6 +469,12 @@
   </si>
   <si>
     <t>s</t>
+  </si>
+  <si>
+    <t>~</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -3027,7 +3033,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30439A0C-B9B0-4751-993E-75FEF8030A87}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
@@ -4034,7 +4040,7 @@
         <v>30</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>4</v>
+        <v>71</v>
       </c>
       <c r="H14" s="12" t="s">
         <v>4</v>
@@ -4082,11 +4088,11 @@
       <c r="Y14" s="7"/>
       <c r="AA14" t="str">
         <f t="shared" si="0"/>
-        <v>#    :  K:    :    #</v>
+        <v>#    :o K:    :    #</v>
       </c>
       <c r="AB14" t="str">
         <f t="shared" si="1"/>
-        <v>'#    :  K:    :    #',</v>
+        <v>'#    :o K:    :    #',</v>
       </c>
     </row>
     <row r="15" spans="1:28" x14ac:dyDescent="0.25">
@@ -17685,7 +17691,7 @@
         <v>4</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>4</v>
+        <v>69</v>
       </c>
       <c r="L11" s="12" t="s">
         <v>4</v>
@@ -17721,11 +17727,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve">                    </v>
+        <v xml:space="preserve">          s         </v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>'                    ',</v>
+        <v>'          s         ',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">
@@ -18624,8 +18630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69EE1C29-EB6B-4425-BBBF-BA7C396F9AF9}">
   <dimension ref="A1:AB30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P11" sqref="P11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AA1" sqref="AA1:AA20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19358,13 +19364,13 @@
         <v>24</v>
       </c>
       <c r="P10" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="Q10" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="R10" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="S10" s="12" t="s">
         <v>24</v>
@@ -19379,11 +19385,11 @@
       <c r="Y10" s="7"/>
       <c r="AA10" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> FFFFFFFFFFFFFF___FF</v>
+        <v xml:space="preserve"> FFFFFFFFFFFFFF~~~FF</v>
       </c>
       <c r="AB10" t="str">
         <f t="shared" si="1"/>
-        <v>' FFFFFFFFFFFFFF___FF',</v>
+        <v>' FFFFFFFFFFFFFF~~~FF',</v>
       </c>
     </row>
     <row r="11" spans="1:28" x14ac:dyDescent="0.25">
@@ -19433,13 +19439,13 @@
         <v>24</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="Q11" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="S11" s="12" t="s">
         <v>24</v>
@@ -19454,11 +19460,11 @@
       <c r="Y11" s="7"/>
       <c r="AA11" t="str">
         <f t="shared" si="0"/>
-        <v xml:space="preserve"> FFFFFFFFFFFFFF___FF</v>
+        <v xml:space="preserve"> FFFFFFFFFFFFFF~~~FF</v>
       </c>
       <c r="AB11" t="str">
         <f t="shared" si="1"/>
-        <v>' FFFFFFFFFFFFFF___FF',</v>
+        <v>' FFFFFFFFFFFFFF~~~FF',</v>
       </c>
     </row>
     <row r="12" spans="1:28" x14ac:dyDescent="0.25">

</xml_diff>